<commit_message>
new result for multi ports
</commit_message>
<xml_diff>
--- a/assets/data/DualRomRead.xlsx
+++ b/assets/data/DualRomRead.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="1180" windowWidth="27340" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Resource Usage</t>
   </si>
@@ -65,10 +65,19 @@
     <t>NumRoms</t>
   </si>
   <si>
-    <t>failed</t>
-  </si>
-  <si>
     <t>stacked to 32</t>
+  </si>
+  <si>
+    <t>NumPipes = 32</t>
+  </si>
+  <si>
+    <t>stacked to 16</t>
+  </si>
+  <si>
+    <t>failed: space</t>
+  </si>
+  <si>
+    <t>failed: timing</t>
   </si>
 </sst>
 </file>
@@ -76,7 +85,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -140,41 +149,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -456,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H19"/>
+  <dimension ref="A3:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,36 +484,36 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="5" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -506,13 +521,13 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>2.4500000000000001E-2</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>3.9E-2</v>
       </c>
       <c r="G6">
@@ -523,13 +538,13 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="2">
         <v>6.6299999999999998E-2</v>
       </c>
       <c r="G7">
@@ -537,220 +552,379 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <f>D7/D6</f>
         <v>1.0204081632653061</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7">
-        <f t="shared" ref="E8:G8" si="0">F7/F6</f>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
+        <f t="shared" ref="F8:G8" si="0">F7/F6</f>
         <v>1.7</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>1.9680597630740284</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="10" t="s">
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="11">
+      <c r="B13" s="7">
         <f>64/C13</f>
         <v>64</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="10">
         <v>1</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="8">
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="17">
         <v>0</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="8">
         <v>1.7805</v>
       </c>
-      <c r="G13" s="14" t="s">
-        <v>13</v>
+      <c r="G13" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="11">
+      <c r="B14" s="7">
         <f t="shared" ref="B14:B19" si="1">64/C14</f>
         <v>32</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="7">
         <v>2</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="17">
         <v>5.6599999999999998E-2</v>
       </c>
-      <c r="E14" s="12">
-        <v>0</v>
-      </c>
-      <c r="F14" s="12">
+      <c r="E14" s="17"/>
+      <c r="F14" s="17">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="7">
         <v>129.40820299999999</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="11">
+      <c r="A15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="7">
         <v>4</v>
       </c>
-      <c r="D15" s="12">
-        <v>5.6599999999999998E-2</v>
-      </c>
-      <c r="E15" s="12">
-        <v>0</v>
-      </c>
-      <c r="F15" s="12">
-        <v>0.93559999999999999</v>
-      </c>
-      <c r="G15" s="13">
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="9">
         <v>117.655518</v>
       </c>
+      <c r="H15">
+        <f>G15/G14</f>
+        <v>0.90918129819019289</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="11">
+      <c r="A16" s="12"/>
+      <c r="B16" s="7">
         <f>64/C16</f>
         <v>8</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="7">
         <v>8</v>
       </c>
-      <c r="D16" s="12">
-        <v>5.6599999999999998E-2</v>
-      </c>
-      <c r="E16" s="12">
-        <v>0</v>
-      </c>
-      <c r="F16" s="12">
-        <v>0.93559999999999999</v>
-      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
       <c r="G16">
         <v>103.65722700000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="11">
+      <c r="H16">
+        <f>G16/G14</f>
+        <v>0.80100970878948086</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="7">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="7">
         <v>16</v>
       </c>
-      <c r="D17" s="12">
-        <v>5.6599999999999998E-2</v>
-      </c>
-      <c r="E17" s="12">
-        <v>0</v>
-      </c>
-      <c r="F17" s="12">
-        <v>0.93559999999999999</v>
-      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
       <c r="G17">
         <v>94.335082999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="11">
+      <c r="H17">
+        <f>G17/G14</f>
+        <v>0.72897297708399522</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="7">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="7">
         <v>32</v>
       </c>
-      <c r="D18" s="12">
-        <v>5.6599999999999998E-2</v>
-      </c>
-      <c r="E18" s="12">
-        <v>0</v>
-      </c>
-      <c r="F18" s="12">
-        <v>0.93559999999999999</v>
-      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
       <c r="G18">
         <v>90.839478</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="11">
+      <c r="H18">
+        <f>G18/G14</f>
+        <v>0.70196074046403389</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="7">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="7">
         <v>64</v>
       </c>
-      <c r="D19" s="12">
-        <v>5.6599999999999998E-2</v>
-      </c>
-      <c r="E19" s="12">
-        <v>0</v>
-      </c>
-      <c r="F19" s="12">
-        <v>0.93559999999999999</v>
-      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
       <c r="G19">
         <v>89.223511000000002</v>
       </c>
+      <c r="H19">
+        <f>G19/G14</f>
+        <v>0.68947337905619488</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C22" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="7">
+        <f>32/C25</f>
+        <v>32</v>
+      </c>
+      <c r="C25" s="11">
+        <v>1</v>
+      </c>
+      <c r="D25" s="8">
+        <v>4.5900000000000003E-2</v>
+      </c>
+      <c r="E25" s="17">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.9093</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="7">
+        <f t="shared" ref="B26:B30" si="2">32/C26</f>
+        <v>16</v>
+      </c>
+      <c r="C26" s="7">
+        <v>2</v>
+      </c>
+      <c r="D26" s="17">
+        <v>4.02E-2</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17">
+        <v>0.47320000000000001</v>
+      </c>
+      <c r="G26" s="7">
+        <v>64.330200000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="7">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="C27" s="7">
+        <v>4</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="9">
+        <v>64.744750999999994</v>
+      </c>
+      <c r="H27">
+        <f>G27/G26</f>
+        <v>1.0064441117857552</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="12"/>
+      <c r="B28" s="7">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="C28" s="7">
+        <v>8</v>
+      </c>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28">
+        <v>63.340088000000002</v>
+      </c>
+      <c r="H28">
+        <f>G28/G26</f>
+        <v>0.98460890841315585</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="12"/>
+      <c r="B29" s="7">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="C29" s="7">
+        <v>16</v>
+      </c>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29">
+        <v>63.648314999999997</v>
+      </c>
+      <c r="H29">
+        <f>G29/G26</f>
+        <v>0.98940023503735397</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="12"/>
+      <c r="B30" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C30" s="7">
+        <v>32</v>
+      </c>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30">
+        <v>63.893188000000002</v>
+      </c>
+      <c r="H30">
+        <f>G30/G26</f>
+        <v>0.99320673649390179</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="18">
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="F26:F30"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="E25:E30"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="C3:G3"/>
@@ -758,6 +932,9 @@
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E13:E19"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="F14:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>